<commit_message>
Ajusta espec demanda TCE
</commit_message>
<xml_diff>
--- a/espec018_recursos-acordo-judicial-vale/static/template_demanda_TCE.xlsx
+++ b/espec018_recursos-acordo-judicial-vale/static/template_demanda_TCE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\.CGE\transparencia-mg\especificacoes-portal-transparencia\espec018_recursos-acordo-judicial-vale\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883E4B25-B9E1-4249-B7AC-20D8DE298D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54291645-F66B-4431-BAEA-8245FE0FEC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28692" yWindow="-108" windowWidth="20712" windowHeight="11016" tabRatio="747" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28692" yWindow="-108" windowWidth="20712" windowHeight="11016" tabRatio="747" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pesquisa Básica Opcao 1 " sheetId="19" state="hidden" r:id="rId1"/>
@@ -221,9 +221,6 @@
     <t>Inscrição em Restos a Pagar</t>
   </si>
   <si>
-    <t>Valor Inscrito:</t>
-  </si>
-  <si>
     <t>Liquidação em Restos a Pagar</t>
   </si>
   <si>
@@ -279,9 +276,6 @@
   </si>
   <si>
     <t>Detalhar</t>
-  </si>
-  <si>
-    <t>Tipo de Inscrição:</t>
   </si>
   <si>
     <t>Valor Liquidado RP</t>
@@ -554,6 +548,12 @@
   </si>
   <si>
     <t>Unidade Executora</t>
+  </si>
+  <si>
+    <t>Valor :</t>
+  </si>
+  <si>
+    <t>Descrição:</t>
   </si>
 </sst>
 </file>
@@ -2620,9 +2620,6 @@
     <xf numFmtId="0" fontId="26" fillId="2" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="31" fillId="5" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2711,6 +2708,9 @@
     <xf numFmtId="8" fontId="24" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2732,65 +2732,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="4" fontId="25" fillId="2" borderId="110" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="25" fillId="2" borderId="114" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="91" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="25" fillId="2" borderId="26" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="25" fillId="2" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="25" fillId="2" borderId="106" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2833,6 +2779,54 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="25" fillId="2" borderId="110" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="25" fillId="2" borderId="114" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="91" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="25" fillId="2" borderId="106" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify"/>
@@ -2969,8 +2963,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -23545,7 +23545,7 @@
     <row r="14" spans="2:17" ht="9.75" customHeight="1"/>
     <row r="15" spans="2:17" ht="28.5" customHeight="1">
       <c r="B15" s="125" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="125"/>
       <c r="D15" s="125"/>
@@ -23582,7 +23582,7 @@
     </row>
     <row r="17" spans="2:17" ht="11.25" customHeight="1">
       <c r="B17" s="41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="37"/>
@@ -23731,7 +23731,7 @@
     </row>
     <row r="39" spans="2:17" ht="32.25" customHeight="1" thickBot="1">
       <c r="B39" s="127" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39" s="127"/>
       <c r="D39" s="127"/>
@@ -23745,7 +23745,7 @@
       </c>
       <c r="K39" s="126"/>
       <c r="L39" s="126" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M39" s="126"/>
       <c r="N39" s="126" t="s">
@@ -23753,7 +23753,7 @@
       </c>
       <c r="O39" s="126"/>
       <c r="P39" s="126" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q39" s="126"/>
     </row>
@@ -23834,7 +23834,7 @@
   <dimension ref="B1:Q30"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -23933,60 +23933,60 @@
       <c r="Q5" s="37"/>
     </row>
     <row r="6" spans="2:17" ht="15" thickBot="1">
-      <c r="B6" s="149" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="150"/>
-      <c r="D6" s="150"/>
-      <c r="E6" s="151"/>
+      <c r="B6" s="131" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="133"/>
     </row>
     <row r="7" spans="2:17" ht="27.6">
       <c r="B7" s="85" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="84" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="84" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="84" t="s">
-        <v>83</v>
-      </c>
       <c r="E7" s="83" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:17" ht="33.75" customHeight="1">
-      <c r="B8" s="152" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="153"/>
-      <c r="D8" s="153"/>
-      <c r="E8" s="154"/>
+      <c r="B8" s="134" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="135"/>
+      <c r="D8" s="135"/>
+      <c r="E8" s="136"/>
     </row>
     <row r="9" spans="2:17" ht="41.25" customHeight="1">
-      <c r="B9" s="152" t="s">
+      <c r="B9" s="134" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="135"/>
+      <c r="D9" s="137" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="138"/>
+      <c r="F9" s="121" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="153"/>
-      <c r="D9" s="155" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="156"/>
-      <c r="F9" s="208" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="97"/>
-      <c r="H9" s="97"/>
-      <c r="I9" s="97"/>
-      <c r="J9" s="97"/>
-      <c r="K9" s="97"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
     </row>
     <row r="10" spans="2:17" ht="69" customHeight="1" thickBot="1">
-      <c r="B10" s="157" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="158"/>
-      <c r="D10" s="158"/>
-      <c r="E10" s="159"/>
+      <c r="B10" s="139" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="140"/>
+      <c r="D10" s="140"/>
+      <c r="E10" s="141"/>
     </row>
     <row r="11" spans="2:17" ht="15" thickBot="1">
       <c r="B11" s="82"/>
@@ -23995,12 +23995,12 @@
       <c r="E11" s="82"/>
     </row>
     <row r="12" spans="2:17" ht="15" thickBot="1">
-      <c r="B12" s="160" t="s">
+      <c r="B12" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="161"/>
-      <c r="D12" s="161"/>
-      <c r="E12" s="162"/>
+      <c r="C12" s="143"/>
+      <c r="D12" s="143"/>
+      <c r="E12" s="144"/>
     </row>
     <row r="13" spans="2:17">
       <c r="B13" s="76" t="s">
@@ -24009,10 +24009,10 @@
       <c r="C13" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="144" t="s">
+      <c r="D13" s="145" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="145"/>
+      <c r="E13" s="146"/>
     </row>
     <row r="14" spans="2:17">
       <c r="B14" s="81">
@@ -24021,10 +24021,10 @@
       <c r="C14" s="80">
         <v>196</v>
       </c>
-      <c r="D14" s="135" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" s="136"/>
+      <c r="D14" s="129" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="130"/>
     </row>
     <row r="15" spans="2:17">
       <c r="B15" s="81">
@@ -24033,10 +24033,10 @@
       <c r="C15" s="80">
         <v>241</v>
       </c>
-      <c r="D15" s="135" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="136"/>
+      <c r="D15" s="129" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="130"/>
     </row>
     <row r="16" spans="2:17" ht="15" thickBot="1">
       <c r="B16" s="79" t="s">
@@ -24044,7 +24044,7 @@
       </c>
       <c r="C16" s="78"/>
       <c r="D16" s="77"/>
-      <c r="E16" s="98">
+      <c r="E16" s="97">
         <v>90427000</v>
       </c>
     </row>
@@ -24055,12 +24055,12 @@
       <c r="E17" s="86"/>
     </row>
     <row r="18" spans="2:8" ht="21.75" customHeight="1" thickBot="1">
-      <c r="B18" s="146" t="s">
+      <c r="B18" s="147" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="147"/>
-      <c r="D18" s="147"/>
-      <c r="E18" s="148"/>
+      <c r="C18" s="148"/>
+      <c r="D18" s="148"/>
+      <c r="E18" s="149"/>
     </row>
     <row r="19" spans="2:8">
       <c r="B19" s="76" t="s">
@@ -24069,10 +24069,10 @@
       <c r="C19" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="144" t="s">
+      <c r="D19" s="145" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="145"/>
+      <c r="E19" s="146"/>
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="81">
@@ -24081,10 +24081,10 @@
       <c r="C20" s="80">
         <v>188</v>
       </c>
-      <c r="D20" s="135" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="136"/>
+      <c r="D20" s="129" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="130"/>
     </row>
     <row r="21" spans="2:8">
       <c r="B21" s="81">
@@ -24093,10 +24093,10 @@
       <c r="C21" s="80">
         <v>189</v>
       </c>
-      <c r="D21" s="135" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21" s="136"/>
+      <c r="D21" s="129" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="130"/>
     </row>
     <row r="22" spans="2:8" ht="15" customHeight="1">
       <c r="B22" s="81">
@@ -24105,10 +24105,10 @@
       <c r="C22" s="80">
         <v>203</v>
       </c>
-      <c r="D22" s="135" t="s">
-        <v>92</v>
-      </c>
-      <c r="E22" s="136"/>
+      <c r="D22" s="129" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="130"/>
     </row>
     <row r="23" spans="2:8" ht="20.399999999999999" customHeight="1" thickBot="1">
       <c r="B23" s="81">
@@ -24117,10 +24117,10 @@
       <c r="C23" s="80">
         <v>214</v>
       </c>
-      <c r="D23" s="135" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" s="136"/>
+      <c r="D23" s="129" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="130"/>
     </row>
     <row r="24" spans="2:8" ht="15" thickBot="1">
       <c r="B24" s="74" t="s">
@@ -24128,83 +24128,92 @@
       </c>
       <c r="C24" s="73"/>
       <c r="D24" s="72"/>
-      <c r="E24" s="99" t="s">
-        <v>94</v>
+      <c r="E24" s="98" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15" thickBot="1"/>
     <row r="26" spans="2:8" ht="15" thickBot="1">
-      <c r="B26" s="137" t="s">
+      <c r="B26" s="156" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="138"/>
-      <c r="D26" s="138"/>
-      <c r="E26" s="139"/>
+      <c r="C26" s="157"/>
+      <c r="D26" s="157"/>
+      <c r="E26" s="158"/>
     </row>
     <row r="27" spans="2:8" ht="15" customHeight="1" thickBot="1">
       <c r="B27" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="89" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="140" t="s">
-        <v>52</v>
-      </c>
-      <c r="E27" s="141"/>
-      <c r="F27" s="133" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" s="134"/>
-      <c r="H27" s="134"/>
+      <c r="C27" s="208" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="206" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="207"/>
+      <c r="F27" s="154" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" s="155"/>
+      <c r="H27" s="155"/>
     </row>
     <row r="28" spans="2:8" ht="24">
-      <c r="B28" s="100">
+      <c r="B28" s="99">
         <v>44932</v>
       </c>
-      <c r="C28" s="101" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="142">
+      <c r="C28" s="100" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="159">
         <v>93983888.390000001</v>
       </c>
-      <c r="E28" s="143"/>
-      <c r="F28" s="133"/>
-      <c r="G28" s="134"/>
-      <c r="H28" s="134"/>
+      <c r="E28" s="160"/>
+      <c r="F28" s="154"/>
+      <c r="G28" s="155"/>
+      <c r="H28" s="155"/>
     </row>
     <row r="29" spans="2:8" ht="24">
-      <c r="B29" s="102">
+      <c r="B29" s="101">
         <v>45295</v>
       </c>
-      <c r="C29" s="103" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="129">
+      <c r="C29" s="102" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="150">
         <v>84674309.719999999</v>
       </c>
-      <c r="E29" s="130"/>
-      <c r="F29" s="133"/>
-      <c r="G29" s="134"/>
-      <c r="H29" s="134"/>
+      <c r="E29" s="151"/>
+      <c r="F29" s="154"/>
+      <c r="G29" s="155"/>
+      <c r="H29" s="155"/>
     </row>
     <row r="30" spans="2:8" ht="24.6" thickBot="1">
-      <c r="B30" s="104">
+      <c r="B30" s="103">
         <v>45376</v>
       </c>
-      <c r="C30" s="105" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="131">
+      <c r="C30" s="104" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="152">
         <v>-24000000</v>
       </c>
-      <c r="E30" s="132"/>
-      <c r="F30" s="133"/>
-      <c r="G30" s="134"/>
-      <c r="H30" s="134"/>
+      <c r="E30" s="153"/>
+      <c r="F30" s="154"/>
+      <c r="G30" s="155"/>
+      <c r="H30" s="155"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F27:H30"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B8:E8"/>
@@ -24217,15 +24226,6 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F27:H30"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -24237,7 +24237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BBDAE66-B66A-48DA-848C-69A723A60232}">
   <dimension ref="B1:Q42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
@@ -24258,22 +24258,22 @@
     </row>
     <row r="6" spans="2:17" ht="9.75" hidden="1" customHeight="1"/>
     <row r="7" spans="2:17" ht="36.75" hidden="1" customHeight="1">
-      <c r="B7" s="163"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="163"/>
-      <c r="H7" s="163"/>
-      <c r="I7" s="163"/>
-      <c r="J7" s="163"/>
-      <c r="K7" s="163"/>
-      <c r="L7" s="163"/>
-      <c r="M7" s="163"/>
-      <c r="N7" s="163"/>
-      <c r="O7" s="163"/>
-      <c r="P7" s="163"/>
-      <c r="Q7" s="163"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="161"/>
+      <c r="E7" s="161"/>
+      <c r="F7" s="161"/>
+      <c r="G7" s="161"/>
+      <c r="H7" s="161"/>
+      <c r="I7" s="161"/>
+      <c r="J7" s="161"/>
+      <c r="K7" s="161"/>
+      <c r="L7" s="161"/>
+      <c r="M7" s="161"/>
+      <c r="N7" s="161"/>
+      <c r="O7" s="161"/>
+      <c r="P7" s="161"/>
+      <c r="Q7" s="161"/>
     </row>
     <row r="8" spans="2:17" ht="12.75" customHeight="1">
       <c r="B8" s="67"/>
@@ -24361,12 +24361,12 @@
     </row>
     <row r="13" spans="2:17" ht="15" thickBot="1"/>
     <row r="14" spans="2:17">
-      <c r="B14" s="164" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="165"/>
-      <c r="E14" s="166"/>
+      <c r="B14" s="162" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="163"/>
+      <c r="D14" s="163"/>
+      <c r="E14" s="164"/>
     </row>
     <row r="15" spans="2:17" ht="15" thickBot="1">
       <c r="B15" s="71" t="s">
@@ -24379,195 +24379,195 @@
         <v>48</v>
       </c>
       <c r="E15" s="68" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="2:17" ht="15" thickBot="1">
-      <c r="B16" s="106">
+      <c r="B16" s="105">
         <v>44641</v>
       </c>
-      <c r="C16" s="107">
+      <c r="C16" s="106">
         <v>3</v>
       </c>
-      <c r="D16" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" s="108">
+      <c r="D16" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="107">
         <v>-690092.97</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="15" thickBot="1">
-      <c r="B17" s="106">
+      <c r="B17" s="105">
         <v>44641</v>
       </c>
-      <c r="C17" s="107">
+      <c r="C17" s="106">
         <v>60</v>
       </c>
-      <c r="D17" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E17" s="109">
+      <c r="D17" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="108">
         <v>690092.97</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1">
-      <c r="B18" s="106">
+      <c r="B18" s="105">
         <v>44642</v>
       </c>
-      <c r="C18" s="107">
+      <c r="C18" s="106">
         <v>61</v>
       </c>
-      <c r="D18" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E18" s="109">
+      <c r="D18" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="108">
         <v>690092.07</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1">
-      <c r="B19" s="106">
+      <c r="B19" s="105">
         <v>44680</v>
       </c>
-      <c r="C19" s="107">
+      <c r="C19" s="106">
         <v>134</v>
       </c>
-      <c r="D19" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E19" s="109">
+      <c r="D19" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="108">
         <v>223201.87</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="15" thickBot="1">
-      <c r="B20" s="106">
+      <c r="B20" s="105">
         <v>44698</v>
       </c>
-      <c r="C20" s="107">
+      <c r="C20" s="106">
         <v>163</v>
       </c>
-      <c r="D20" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" s="109">
+      <c r="D20" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="108">
         <v>241326.76</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="15" thickBot="1">
-      <c r="B21" s="106">
+      <c r="B21" s="105">
         <v>44735</v>
       </c>
-      <c r="C21" s="107">
+      <c r="C21" s="106">
         <v>237</v>
       </c>
-      <c r="D21" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21" s="109">
+      <c r="D21" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="108">
         <v>645585.44999999995</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="15" thickBot="1">
-      <c r="B22" s="106">
+      <c r="B22" s="105">
         <v>44767</v>
       </c>
-      <c r="C22" s="107">
+      <c r="C22" s="106">
         <v>306</v>
       </c>
-      <c r="D22" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" s="109">
+      <c r="D22" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="108">
         <v>611167.96</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="15" thickBot="1">
-      <c r="B23" s="106">
+      <c r="B23" s="105">
         <v>44790</v>
       </c>
-      <c r="C23" s="107">
+      <c r="C23" s="106">
         <v>342</v>
       </c>
-      <c r="D23" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E23" s="109">
+      <c r="D23" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="108">
         <v>734337.23</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="15" thickBot="1">
-      <c r="B24" s="106">
+      <c r="B24" s="105">
         <v>44826</v>
       </c>
-      <c r="C24" s="107">
+      <c r="C24" s="106">
         <v>402</v>
       </c>
-      <c r="D24" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E24" s="109">
+      <c r="D24" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="108">
         <v>864643.87</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15" thickBot="1">
-      <c r="B25" s="106">
+      <c r="B25" s="105">
         <v>44858</v>
       </c>
-      <c r="C25" s="107">
+      <c r="C25" s="106">
         <v>493</v>
       </c>
-      <c r="D25" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" s="109">
+      <c r="D25" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="108">
         <v>1022841.39</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="15" thickBot="1">
-      <c r="B26" s="106">
+      <c r="B26" s="105">
         <v>44893</v>
       </c>
-      <c r="C26" s="107">
+      <c r="C26" s="106">
         <v>588</v>
       </c>
-      <c r="D26" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E26" s="109">
+      <c r="D26" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="108">
         <v>943408.64000000001</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="15" thickBot="1">
-      <c r="B27" s="106">
+      <c r="B27" s="105">
         <v>44918</v>
       </c>
-      <c r="C27" s="107">
+      <c r="C27" s="106">
         <v>651</v>
       </c>
-      <c r="D27" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E27" s="109">
+      <c r="D27" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="108">
         <v>1476861.58</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="15" thickBot="1">
-      <c r="B28" s="167" t="s">
-        <v>99</v>
-      </c>
-      <c r="C28" s="168"/>
-      <c r="D28" s="169"/>
-      <c r="E28" s="110">
+      <c r="B28" s="165" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="166"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="109">
         <v>7453466.8200000003</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="15" thickBot="1"/>
     <row r="30" spans="2:8">
-      <c r="B30" s="170" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="171"/>
-      <c r="D30" s="171"/>
-      <c r="E30" s="172"/>
+      <c r="B30" s="168" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="169"/>
+      <c r="D30" s="169"/>
+      <c r="E30" s="170"/>
     </row>
     <row r="31" spans="2:8" ht="15" thickBot="1">
       <c r="B31" s="71" t="s">
@@ -24580,188 +24580,188 @@
         <v>48</v>
       </c>
       <c r="E31" s="68" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="15" customHeight="1" thickBot="1">
-      <c r="B32" s="106" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" s="107">
+      <c r="B32" s="105" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="106">
         <v>31</v>
       </c>
-      <c r="D32" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E32" s="109">
+      <c r="D32" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="108">
         <v>1238097.06</v>
       </c>
-      <c r="F32" s="176" t="s">
-        <v>101</v>
-      </c>
-      <c r="G32" s="177"/>
-      <c r="H32" s="177"/>
+      <c r="F32" s="174" t="s">
+        <v>99</v>
+      </c>
+      <c r="G32" s="175"/>
+      <c r="H32" s="175"/>
     </row>
     <row r="33" spans="2:8" ht="15" thickBot="1">
-      <c r="B33" s="106">
+      <c r="B33" s="105">
         <v>44998</v>
       </c>
-      <c r="C33" s="107">
+      <c r="C33" s="106">
         <v>73</v>
       </c>
-      <c r="D33" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E33" s="109">
+      <c r="D33" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="108">
         <v>1502509.18</v>
       </c>
-      <c r="F33" s="176"/>
-      <c r="G33" s="177"/>
-      <c r="H33" s="177"/>
+      <c r="F33" s="174"/>
+      <c r="G33" s="175"/>
+      <c r="H33" s="175"/>
     </row>
     <row r="34" spans="2:8" ht="15" thickBot="1">
-      <c r="B34" s="106">
+      <c r="B34" s="105">
         <v>45027</v>
       </c>
-      <c r="C34" s="107">
+      <c r="C34" s="106">
         <v>99</v>
       </c>
-      <c r="D34" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E34" s="109">
+      <c r="D34" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="108">
         <v>347103.23</v>
       </c>
-      <c r="F34" s="176"/>
-      <c r="G34" s="177"/>
-      <c r="H34" s="177"/>
+      <c r="F34" s="174"/>
+      <c r="G34" s="175"/>
+      <c r="H34" s="175"/>
     </row>
     <row r="35" spans="2:8" ht="15" thickBot="1">
-      <c r="B35" s="106">
+      <c r="B35" s="105">
         <v>45036</v>
       </c>
-      <c r="C35" s="107">
+      <c r="C35" s="106">
         <v>122</v>
       </c>
-      <c r="D35" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E35" s="109">
+      <c r="D35" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="108">
         <v>1252620.23</v>
       </c>
-      <c r="F35" s="176"/>
-      <c r="G35" s="177"/>
-      <c r="H35" s="177"/>
+      <c r="F35" s="174"/>
+      <c r="G35" s="175"/>
+      <c r="H35" s="175"/>
     </row>
     <row r="36" spans="2:8" ht="15" thickBot="1">
-      <c r="B36" s="106">
+      <c r="B36" s="105">
         <v>45063</v>
       </c>
-      <c r="C36" s="107">
+      <c r="C36" s="106">
         <v>157</v>
       </c>
-      <c r="D36" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E36" s="109">
+      <c r="D36" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="108">
         <v>907859.51</v>
       </c>
-      <c r="F36" s="176"/>
-      <c r="G36" s="177"/>
-      <c r="H36" s="177"/>
+      <c r="F36" s="174"/>
+      <c r="G36" s="175"/>
+      <c r="H36" s="175"/>
     </row>
     <row r="37" spans="2:8" ht="15" thickBot="1">
-      <c r="B37" s="106">
+      <c r="B37" s="105">
         <v>45104</v>
       </c>
-      <c r="C37" s="107">
+      <c r="C37" s="106">
         <v>186</v>
       </c>
-      <c r="D37" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E37" s="109">
+      <c r="D37" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="108">
         <v>2867391.06</v>
       </c>
-      <c r="F37" s="176"/>
-      <c r="G37" s="177"/>
-      <c r="H37" s="177"/>
+      <c r="F37" s="174"/>
+      <c r="G37" s="175"/>
+      <c r="H37" s="175"/>
     </row>
     <row r="38" spans="2:8" ht="15" thickBot="1">
-      <c r="B38" s="106">
+      <c r="B38" s="105">
         <v>45135</v>
       </c>
-      <c r="C38" s="107">
+      <c r="C38" s="106">
         <v>203</v>
       </c>
-      <c r="D38" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E38" s="109">
+      <c r="D38" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="108">
         <v>1193998.3999999999</v>
       </c>
-      <c r="F38" s="176"/>
-      <c r="G38" s="177"/>
-      <c r="H38" s="177"/>
+      <c r="F38" s="174"/>
+      <c r="G38" s="175"/>
+      <c r="H38" s="175"/>
     </row>
     <row r="39" spans="2:8" ht="15" thickBot="1">
-      <c r="B39" s="106">
+      <c r="B39" s="105">
         <v>45167</v>
       </c>
-      <c r="C39" s="107">
+      <c r="C39" s="106">
         <v>210</v>
       </c>
-      <c r="D39" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E39" s="109">
+      <c r="D39" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" s="108">
         <v>1395383.95</v>
       </c>
-      <c r="F39" s="176"/>
-      <c r="G39" s="177"/>
-      <c r="H39" s="177"/>
+      <c r="F39" s="174"/>
+      <c r="G39" s="175"/>
+      <c r="H39" s="175"/>
     </row>
     <row r="40" spans="2:8" ht="15" thickBot="1">
-      <c r="B40" s="106">
+      <c r="B40" s="105">
         <v>45190</v>
       </c>
-      <c r="C40" s="107">
+      <c r="C40" s="106">
         <v>15</v>
       </c>
-      <c r="D40" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E40" s="109">
+      <c r="D40" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" s="108">
         <v>-1395383.95</v>
       </c>
-      <c r="F40" s="176"/>
-      <c r="G40" s="177"/>
-      <c r="H40" s="177"/>
+      <c r="F40" s="174"/>
+      <c r="G40" s="175"/>
+      <c r="H40" s="175"/>
     </row>
     <row r="41" spans="2:8" ht="15" thickBot="1">
-      <c r="B41" s="106">
+      <c r="B41" s="105">
         <v>45315</v>
       </c>
-      <c r="C41" s="107">
+      <c r="C41" s="106">
         <v>39</v>
       </c>
-      <c r="D41" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="E41" s="109">
+      <c r="D41" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" s="108">
         <v>695891.64</v>
       </c>
-      <c r="F41" s="176"/>
-      <c r="G41" s="177"/>
-      <c r="H41" s="177"/>
+      <c r="F41" s="174"/>
+      <c r="G41" s="175"/>
+      <c r="H41" s="175"/>
     </row>
     <row r="42" spans="2:8" ht="15" thickBot="1">
-      <c r="B42" s="173" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" s="174"/>
-      <c r="D42" s="175"/>
-      <c r="E42" s="111">
+      <c r="B42" s="171" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="172"/>
+      <c r="D42" s="173"/>
+      <c r="E42" s="110">
         <v>10005470.310000001</v>
       </c>
     </row>
@@ -24867,221 +24867,221 @@
       <c r="Q7" s="37"/>
     </row>
     <row r="10" spans="2:17" ht="21.75" customHeight="1">
-      <c r="B10" s="178" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="179"/>
-      <c r="D10" s="179"/>
-      <c r="E10" s="179"/>
-      <c r="F10" s="179"/>
+      <c r="B10" s="176" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="177"/>
+      <c r="D10" s="177"/>
+      <c r="E10" s="177"/>
+      <c r="F10" s="177"/>
     </row>
     <row r="11" spans="2:17" ht="28.2" thickBot="1">
-      <c r="B11" s="112" t="s">
+      <c r="B11" s="111" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="112" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="113" t="s">
+      <c r="D11" s="112" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="114" t="s">
+      <c r="E11" s="113" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="115" t="s">
-        <v>67</v>
+      <c r="F11" s="114" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="2:17" ht="21.75" customHeight="1" thickBot="1">
-      <c r="B12" s="116">
+      <c r="B12" s="115">
         <v>44643</v>
       </c>
-      <c r="C12" s="117">
+      <c r="C12" s="116">
         <v>106</v>
       </c>
-      <c r="D12" s="117" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="117" t="s">
-        <v>98</v>
-      </c>
-      <c r="F12" s="118">
+      <c r="D12" s="116" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="116" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="117">
         <v>690092.07</v>
       </c>
     </row>
     <row r="13" spans="2:17" ht="21" thickBot="1">
-      <c r="B13" s="106">
+      <c r="B13" s="105">
         <v>44685</v>
       </c>
-      <c r="C13" s="107">
+      <c r="C13" s="106">
         <v>209</v>
       </c>
-      <c r="D13" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F13" s="109">
+      <c r="D13" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="108">
         <v>223201.87</v>
       </c>
     </row>
     <row r="14" spans="2:17" ht="21" thickBot="1">
-      <c r="B14" s="106">
+      <c r="B14" s="105">
         <v>44704</v>
       </c>
-      <c r="C14" s="107">
+      <c r="C14" s="106">
         <v>227</v>
       </c>
-      <c r="D14" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F14" s="109">
+      <c r="D14" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="108">
         <v>241326.76</v>
       </c>
     </row>
     <row r="15" spans="2:17" ht="21" thickBot="1">
-      <c r="B15" s="106">
+      <c r="B15" s="105">
         <v>44741</v>
       </c>
-      <c r="C15" s="107">
+      <c r="C15" s="106">
         <v>333</v>
       </c>
-      <c r="D15" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F15" s="109">
+      <c r="D15" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" s="108">
         <v>645585.44999999995</v>
       </c>
     </row>
     <row r="16" spans="2:17" ht="21" thickBot="1">
-      <c r="B16" s="106">
+      <c r="B16" s="105">
         <v>44769</v>
       </c>
-      <c r="C16" s="107">
+      <c r="C16" s="106">
         <v>401</v>
       </c>
-      <c r="D16" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F16" s="109">
+      <c r="D16" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="108">
         <v>611167.96</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="35.25" customHeight="1" thickBot="1">
-      <c r="B17" s="106">
+      <c r="B17" s="105">
         <v>44797</v>
       </c>
-      <c r="C17" s="107">
+      <c r="C17" s="106">
         <v>438</v>
       </c>
-      <c r="D17" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F17" s="109">
+      <c r="D17" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="108">
         <v>734337.23</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="21" thickBot="1">
-      <c r="B18" s="106">
+      <c r="B18" s="105">
         <v>44827</v>
       </c>
-      <c r="C18" s="107">
+      <c r="C18" s="106">
         <v>494</v>
       </c>
-      <c r="D18" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F18" s="109">
+      <c r="D18" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="108">
         <v>864643.87</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="21" thickBot="1">
-      <c r="B19" s="106">
+      <c r="B19" s="105">
         <v>44860</v>
       </c>
-      <c r="C19" s="107">
+      <c r="C19" s="106">
         <v>604</v>
       </c>
-      <c r="D19" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F19" s="109">
+      <c r="D19" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19" s="108">
         <v>1022841.39</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="21" thickBot="1">
-      <c r="B20" s="106">
+      <c r="B20" s="105">
         <v>44894</v>
       </c>
-      <c r="C20" s="107">
+      <c r="C20" s="106">
         <v>670</v>
       </c>
-      <c r="D20" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F20" s="109">
+      <c r="D20" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" s="108">
         <v>943408.64000000001</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="21" thickBot="1">
-      <c r="B21" s="106">
+      <c r="B21" s="105">
         <v>44923</v>
       </c>
-      <c r="C21" s="107">
+      <c r="C21" s="106">
         <v>741</v>
       </c>
-      <c r="D21" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="109">
+      <c r="D21" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F21" s="108">
         <v>1476861.58</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="15" thickBot="1">
-      <c r="B22" s="173" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="174"/>
-      <c r="D22" s="174"/>
-      <c r="E22" s="175"/>
-      <c r="F22" s="111">
+      <c r="B22" s="171" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="172"/>
+      <c r="D22" s="172"/>
+      <c r="E22" s="173"/>
+      <c r="F22" s="110">
         <v>7453466.8200000003</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="15" thickBot="1"/>
     <row r="24" spans="2:6">
-      <c r="B24" s="170" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="171"/>
-      <c r="D24" s="171"/>
-      <c r="E24" s="171"/>
-      <c r="F24" s="172"/>
+      <c r="B24" s="168" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="169"/>
+      <c r="D24" s="169"/>
+      <c r="E24" s="169"/>
+      <c r="F24" s="170"/>
     </row>
     <row r="25" spans="2:6" ht="28.2" thickBot="1">
       <c r="B25" s="71" t="s">
@@ -25097,136 +25097,136 @@
         <v>48</v>
       </c>
       <c r="F25" s="68" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="21" thickBot="1">
-      <c r="B26" s="119">
+      <c r="B26" s="118">
         <v>44952</v>
       </c>
-      <c r="C26" s="107">
+      <c r="C26" s="106">
         <v>19</v>
       </c>
-      <c r="D26" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F26" s="120">
+      <c r="D26" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="119">
         <v>1238097.06</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="21" thickBot="1">
-      <c r="B27" s="119">
+      <c r="B27" s="118">
         <v>45002</v>
       </c>
-      <c r="C27" s="107">
+      <c r="C27" s="106">
         <v>69</v>
       </c>
-      <c r="D27" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F27" s="120">
+      <c r="D27" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" s="119">
         <v>1502509.18</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="21" thickBot="1">
-      <c r="B28" s="119">
+      <c r="B28" s="118">
         <v>45029</v>
       </c>
-      <c r="C28" s="107">
+      <c r="C28" s="106">
         <v>104</v>
       </c>
-      <c r="D28" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" s="120">
+      <c r="D28" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="119">
         <v>347103.23</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="21" thickBot="1">
-      <c r="B29" s="119">
+      <c r="B29" s="118">
         <v>45041</v>
       </c>
-      <c r="C29" s="107">
+      <c r="C29" s="106">
         <v>140</v>
       </c>
-      <c r="D29" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E29" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F29" s="120">
+      <c r="D29" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="119">
         <v>1252620.23</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="21" thickBot="1">
-      <c r="B30" s="119">
+      <c r="B30" s="118">
         <v>45069</v>
       </c>
-      <c r="C30" s="107">
+      <c r="C30" s="106">
         <v>185</v>
       </c>
-      <c r="D30" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F30" s="120">
+      <c r="D30" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F30" s="119">
         <v>907859.51</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="21" thickBot="1">
-      <c r="B31" s="119">
+      <c r="B31" s="118">
         <v>45107</v>
       </c>
-      <c r="C31" s="107">
+      <c r="C31" s="106">
         <v>286</v>
       </c>
-      <c r="D31" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F31" s="120">
+      <c r="D31" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="119">
         <v>2867391.06</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="21" thickBot="1">
-      <c r="B32" s="119">
+      <c r="B32" s="118">
         <v>45140</v>
       </c>
-      <c r="C32" s="107">
+      <c r="C32" s="106">
         <v>344</v>
       </c>
-      <c r="D32" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="F32" s="120">
+      <c r="D32" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" s="119">
         <v>1193998.3999999999</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="15" thickBot="1">
-      <c r="B33" s="180" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" s="181"/>
-      <c r="D33" s="181"/>
-      <c r="E33" s="182"/>
-      <c r="F33" s="121">
+      <c r="B33" s="178" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="179"/>
+      <c r="D33" s="179"/>
+      <c r="E33" s="180"/>
+      <c r="F33" s="120">
         <v>9309578.6699999999</v>
       </c>
     </row>
@@ -25266,74 +25266,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="70.2" customHeight="1">
-      <c r="A1" s="96" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="96" t="s">
+      <c r="A1" s="95" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="91" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="91" t="s">
+      <c r="D1" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="91" t="s">
+      <c r="F1" s="90" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="90" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="91" t="s">
+      <c r="I1" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="91" t="s">
+      <c r="J1" s="90" t="s">
         <v>73</v>
-      </c>
-      <c r="I1" s="91" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="91" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="36.6" customHeight="1">
-      <c r="A2" s="92"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
+      <c r="A2" s="91"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
     </row>
     <row r="3" spans="1:10" ht="36.6" customHeight="1">
-      <c r="A3" s="95"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
+      <c r="A3" s="94"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
     </row>
     <row r="4" spans="1:10" ht="36.6" customHeight="1">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="93"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -25364,98 +25364,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="70.2" customHeight="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="95" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="95" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="95" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="F1" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="96" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" s="96" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" s="96" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" s="91" t="s">
+      <c r="G1" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="91" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="91" t="s">
+      <c r="H1" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="91" t="s">
+      <c r="J1" s="90" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="90" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="91" t="s">
+      <c r="M1" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="L1" s="91" t="s">
+      <c r="N1" s="90" t="s">
         <v>73</v>
-      </c>
-      <c r="M1" s="91" t="s">
-        <v>74</v>
-      </c>
-      <c r="N1" s="91" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="36.6" customHeight="1">
-      <c r="A2" s="92"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="A2" s="91"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
     </row>
     <row r="3" spans="1:14" ht="36.6" customHeight="1">
-      <c r="A3" s="95"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
+      <c r="A3" s="94"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
+      <c r="L3" s="94"/>
+      <c r="M3" s="94"/>
+      <c r="N3" s="94"/>
     </row>
     <row r="4" spans="1:14" ht="36.6" customHeight="1">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="94"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -25467,7 +25467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2643730C-A887-480C-82C3-06459936A46E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -25508,48 +25508,48 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" thickBot="1">
-      <c r="A6" s="187" t="s">
+      <c r="A6" s="185" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="188"/>
-      <c r="C6" s="188"/>
-      <c r="D6" s="189"/>
-      <c r="E6" s="190" t="s">
+      <c r="B6" s="186"/>
+      <c r="C6" s="186"/>
+      <c r="D6" s="187"/>
+      <c r="E6" s="188" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="191"/>
+      <c r="F6" s="189"/>
       <c r="H6" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" thickBot="1">
-      <c r="A7" s="192" t="s">
+      <c r="A7" s="190" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="193"/>
-      <c r="C7" s="193"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="199">
+      <c r="B7" s="191"/>
+      <c r="C7" s="191"/>
+      <c r="D7" s="192"/>
+      <c r="E7" s="197">
         <f>'Pesquisa básica 1'!X2</f>
         <v>3478961699.73</v>
       </c>
-      <c r="F7" s="200"/>
+      <c r="F7" s="198"/>
       <c r="H7" s="24" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1">
-      <c r="A8" s="183" t="s">
+      <c r="A8" s="181" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="195"/>
-      <c r="C8" s="195"/>
-      <c r="D8" s="184"/>
-      <c r="E8" s="201">
+      <c r="B8" s="193"/>
+      <c r="C8" s="193"/>
+      <c r="D8" s="182"/>
+      <c r="E8" s="199">
         <f>'Pesquisa básica 1'!W15</f>
         <v>720584233.74000001</v>
       </c>
-      <c r="F8" s="202"/>
+      <c r="F8" s="200"/>
       <c r="H8" s="24" t="s">
         <v>14</v>
       </c>
@@ -25561,27 +25561,27 @@
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
       <c r="D9" s="33"/>
-      <c r="E9" s="205">
+      <c r="E9" s="203">
         <f>'Pesquisa básica 1'!X15</f>
         <v>599300000</v>
       </c>
-      <c r="F9" s="206"/>
+      <c r="F9" s="204"/>
       <c r="H9" s="24" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A10" s="196" t="s">
+      <c r="A10" s="194" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="197"/>
-      <c r="C10" s="197"/>
-      <c r="D10" s="198"/>
-      <c r="E10" s="203">
+      <c r="B10" s="195"/>
+      <c r="C10" s="195"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="201">
         <f>'Pesquisa básica 1'!Y15</f>
         <v>599300000</v>
       </c>
-      <c r="F10" s="204"/>
+      <c r="F10" s="202"/>
       <c r="H10" s="24" t="s">
         <v>16</v>
       </c>
@@ -25608,10 +25608,10 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A21" s="187" t="s">
+      <c r="A21" s="185" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="189"/>
+      <c r="B21" s="187"/>
       <c r="C21" s="4">
         <v>2021</v>
       </c>
@@ -25626,11 +25626,11 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A22" s="192" t="str">
+      <c r="A22" s="190" t="str">
         <f>A7</f>
         <v>Repassado ao Estado</v>
       </c>
-      <c r="B22" s="194"/>
+      <c r="B22" s="192"/>
       <c r="C22" s="12">
         <f>E7</f>
         <v>3478961699.73</v>
@@ -25640,11 +25640,11 @@
       <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A23" s="183" t="str">
+      <c r="A23" s="181" t="str">
         <f>A8</f>
         <v>Empenhado</v>
       </c>
-      <c r="B23" s="184"/>
+      <c r="B23" s="182"/>
       <c r="C23" s="2">
         <f>E8</f>
         <v>720584233.74000001</v>
@@ -25654,11 +25654,11 @@
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A24" s="183" t="str">
+      <c r="A24" s="181" t="str">
         <f>A9</f>
         <v>Liquidado</v>
       </c>
-      <c r="B24" s="184"/>
+      <c r="B24" s="182"/>
       <c r="C24" s="2">
         <f>E9</f>
         <v>599300000</v>
@@ -25668,11 +25668,11 @@
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A25" s="183" t="str">
+      <c r="A25" s="181" t="str">
         <f>A10</f>
         <v>Pago</v>
       </c>
-      <c r="B25" s="184"/>
+      <c r="B25" s="182"/>
       <c r="C25" s="2">
         <f>E10</f>
         <v>599300000</v>
@@ -25682,10 +25682,10 @@
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="15" thickBot="1">
-      <c r="A26" s="185" t="s">
+      <c r="A26" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="186"/>
+      <c r="B26" s="184"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7">
         <f>SUM(D22:D25)</f>
@@ -25902,11 +25902,11 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A17" s="185" t="s">
+      <c r="A17" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="207"/>
-      <c r="C17" s="186"/>
+      <c r="B17" s="205"/>
+      <c r="C17" s="184"/>
       <c r="D17" s="7">
         <f>SUM(D11:D16)</f>
         <v>603978445.99666667</v>
@@ -26172,7 +26172,7 @@
     <row r="14" spans="2:17" ht="9.75" customHeight="1"/>
     <row r="15" spans="2:17" ht="39.75" customHeight="1">
       <c r="B15" s="125" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="125"/>
       <c r="D15" s="125"/>
@@ -26209,7 +26209,7 @@
     </row>
     <row r="17" spans="2:17" ht="11.25" customHeight="1">
       <c r="B17" s="41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="37"/>
@@ -26286,7 +26286,7 @@
     </row>
     <row r="53" spans="2:17" ht="32.25" customHeight="1" thickBot="1">
       <c r="B53" s="127" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C53" s="127"/>
       <c r="D53" s="127"/>
@@ -26300,7 +26300,7 @@
       </c>
       <c r="K53" s="126"/>
       <c r="L53" s="126" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M53" s="126"/>
       <c r="N53" s="126" t="s">
@@ -26308,7 +26308,7 @@
       </c>
       <c r="O53" s="126"/>
       <c r="P53" s="126" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q53" s="126"/>
     </row>
@@ -26428,7 +26428,7 @@
     <row r="14" spans="2:17" ht="9.75" customHeight="1"/>
     <row r="15" spans="2:17" ht="39.75" customHeight="1">
       <c r="B15" s="125" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="125"/>
       <c r="D15" s="125"/>
@@ -26465,7 +26465,7 @@
     </row>
     <row r="17" spans="2:17" ht="11.25" customHeight="1">
       <c r="B17" s="41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="37"/>
@@ -26542,7 +26542,7 @@
     </row>
     <row r="53" spans="2:17" ht="32.25" customHeight="1" thickBot="1">
       <c r="B53" s="127" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C53" s="127"/>
       <c r="D53" s="127"/>
@@ -26556,7 +26556,7 @@
       </c>
       <c r="K53" s="126"/>
       <c r="L53" s="126" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M53" s="126"/>
       <c r="N53" s="126" t="s">
@@ -26564,7 +26564,7 @@
       </c>
       <c r="O53" s="126"/>
       <c r="P53" s="126" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q53" s="126"/>
     </row>
@@ -26957,80 +26957,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="70.2" customHeight="1">
-      <c r="A1" s="90" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="90" t="s">
+      <c r="A1" s="89" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="89" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="90" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="90" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="90" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="H1" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="91" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="91" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="91" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="91" t="s">
+      <c r="I1" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="91" t="s">
+      <c r="J1" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="91" t="s">
+      <c r="K1" s="90" t="s">
         <v>73</v>
-      </c>
-      <c r="J1" s="91" t="s">
-        <v>74</v>
-      </c>
-      <c r="K1" s="91" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="36.6" customHeight="1">
-      <c r="A2" s="92"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
+      <c r="A2" s="91"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
     </row>
     <row r="3" spans="1:11" ht="36.6" customHeight="1">
-      <c r="A3" s="95"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
+      <c r="A3" s="94"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
     </row>
     <row r="4" spans="1:11" ht="36.6" customHeight="1">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -27061,92 +27061,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="70.2" customHeight="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="95" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="90" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="96" t="s">
+      <c r="E1" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="96" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" s="91" t="s">
+      <c r="F1" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="91" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="91" t="s">
+      <c r="G1" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="91" t="s">
+      <c r="I1" s="90" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="90" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="91" t="s">
+      <c r="L1" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="91" t="s">
+      <c r="M1" s="90" t="s">
         <v>73</v>
-      </c>
-      <c r="L1" s="91" t="s">
-        <v>74</v>
-      </c>
-      <c r="M1" s="91" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="36.6" customHeight="1">
-      <c r="A2" s="92"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
+      <c r="A2" s="91"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
     </row>
     <row r="3" spans="1:13" ht="36.6" customHeight="1">
-      <c r="A3" s="95"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
+      <c r="A3" s="94"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
+      <c r="L3" s="94"/>
+      <c r="M3" s="94"/>
     </row>
     <row r="4" spans="1:13" ht="36.6" customHeight="1">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="94"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>